<commit_message>
Added comment to "other pains and symptoms"
</commit_message>
<xml_diff>
--- a/app/config/tables/MIF_FAL/forms/MIF_FAL/MIF_FAL.xlsx
+++ b/app/config/tables/MIF_FAL/forms/MIF_FAL/MIF_FAL.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6762710C-565D-4531-BB8B-63308FFC304F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E244BA4B-540B-4919-AA7F-9DE3458683F0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="225">
   <si>
     <t>setting_name</t>
   </si>
@@ -728,6 +728,27 @@
   </si>
   <si>
     <t>DEATHDATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>data('OUTRODUR') == '1'</t>
+  </si>
+  <si>
+    <t>OUTRODURCOM</t>
+  </si>
+  <si>
+    <t>data('OUTROSIMP')</t>
+  </si>
+  <si>
+    <t>OUTROSIMPCOM</t>
+  </si>
+  <si>
+    <t>Which pains</t>
+  </si>
+  <si>
+    <t>Which symptoms</t>
   </si>
 </sst>
 </file>
@@ -932,7 +953,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -976,6 +997,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -1377,11 +1399,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:M90"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C80" sqref="C80"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F87" activeCellId="1" sqref="F83 F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,6 +2283,9 @@
       <c r="B80" t="s">
         <v>46</v>
       </c>
+      <c r="C80" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="28"/>
@@ -2282,91 +2307,151 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="28"/>
-      <c r="D82" t="s">
-        <v>22</v>
-      </c>
-      <c r="E82" t="s">
-        <v>54</v>
-      </c>
-      <c r="F82" t="s">
-        <v>191</v>
-      </c>
-      <c r="G82" t="s">
-        <v>189</v>
-      </c>
-      <c r="H82" t="s">
-        <v>210</v>
+      <c r="B82" t="s">
+        <v>62</v>
+      </c>
+      <c r="C82" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="28"/>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
+        <v>49</v>
+      </c>
+      <c r="F83" t="s">
+        <v>220</v>
+      </c>
+      <c r="G83" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="H83" s="37" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="28"/>
+      <c r="B84" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="28"/>
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" t="s">
+        <v>54</v>
+      </c>
+      <c r="F85" t="s">
+        <v>191</v>
+      </c>
+      <c r="G85" t="s">
+        <v>189</v>
+      </c>
+      <c r="H85" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="28"/>
+      <c r="B86" t="s">
+        <v>62</v>
+      </c>
+      <c r="C86" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="28"/>
+      <c r="D87" t="s">
+        <v>49</v>
+      </c>
+      <c r="F87" t="s">
+        <v>222</v>
+      </c>
+      <c r="G87" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="H87" s="37" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="28"/>
+      <c r="B88" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="28"/>
+      <c r="B89" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6" t="s">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="6"/>
+      <c r="B90" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="34"/>
-      <c r="B85" t="s">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="34"/>
+      <c r="B91" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="34"/>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" t="s">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="34"/>
+      <c r="D92" t="s">
+        <v>22</v>
+      </c>
+      <c r="E92" t="s">
         <v>54</v>
       </c>
-      <c r="F86" t="s">
+      <c r="F92" t="s">
         <v>195</v>
       </c>
-      <c r="G86" t="s">
+      <c r="G92" t="s">
         <v>193</v>
       </c>
-      <c r="H86" t="s">
+      <c r="H92" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="34"/>
-      <c r="B87" t="s">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="34"/>
+      <c r="B93" t="s">
         <v>62</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C93" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="34"/>
-      <c r="D88" t="s">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="34"/>
+      <c r="D94" t="s">
         <v>49</v>
       </c>
-      <c r="F88" t="s">
+      <c r="F94" t="s">
         <v>196</v>
       </c>
-      <c r="G88" t="s">
+      <c r="G94" t="s">
         <v>197</v>
       </c>
-      <c r="H88" t="s">
+      <c r="H94" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="34"/>
-      <c r="B89" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="34"/>
+      <c r="B95" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" t="s">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="34"/>
+      <c r="B96" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3151,16 +3236,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3577,7 +3662,6 @@
         <v>0</v>
       </c>
       <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -3590,7 +3674,6 @@
         <v>0</v>
       </c>
       <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
@@ -3605,31 +3688,35 @@
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
     </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>220</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+    </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="B36" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>65</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" t="b">
-        <v>0</v>
-      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>217</v>
       </c>
       <c r="B38" t="s">
         <v>60</v>
@@ -3640,17 +3727,39 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>200</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>49</v>
       </c>
-      <c r="C39" t="b">
+      <c r="C41" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:F82">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:F84">
     <sortCondition ref="E3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>